<commit_message>
RTM: latest defect list
</commit_message>
<xml_diff>
--- a/src/com/accenture/tmt/Quality_Tracker/newdefects1.xlsx
+++ b/src/com/accenture/tmt/Quality_Tracker/newdefects1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
   <si>
     <t>Priority</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>fixed</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -268,6 +274,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -275,7 +284,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -559,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,39 +585,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -678,8 +687,8 @@
         <v>12</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
+      <c r="F6" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="G6" s="5">
         <v>42234</v>
@@ -701,16 +710,14 @@
         <v>12</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
+      <c r="F7" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="8">
         <v>42234</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -846,7 +853,7 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G13" s="8">
         <v>42234</v>
@@ -964,8 +971,8 @@
         <v>34</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>14</v>
+      <c r="F18" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="G18" s="8">
         <v>42234</v>
@@ -1056,8 +1063,8 @@
         <v>12</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
-        <v>14</v>
+      <c r="F22" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="G22" s="8">
         <v>42234</v>
@@ -1080,7 +1087,7 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="G23" s="8">
         <v>42234</v>
@@ -1125,8 +1132,8 @@
         <v>12</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>14</v>
+      <c r="F25" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="G25" s="8">
         <v>42234</v>

</xml_diff>

<commit_message>
RTM: updated defect list
</commit_message>
<xml_diff>
--- a/src/com/accenture/tmt/Quality_Tracker/newdefects1.xlsx
+++ b/src/com/accenture/tmt/Quality_Tracker/newdefects1.xlsx
@@ -8,7 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$I$31</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
   <si>
     <t>Priority</t>
   </si>
@@ -63,9 +67,6 @@
     <t>Closed</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Contact us page is not updated in LogIN page</t>
   </si>
   <si>
@@ -111,9 +112,6 @@
     <t>Add Employee manually,validations for the fields is not there</t>
   </si>
   <si>
-    <t>For some fields no validations.</t>
-  </si>
-  <si>
     <t>Selecting the admintool tab, Add module should be highlighted and should be navigate to add module page</t>
   </si>
   <si>
@@ -144,22 +142,67 @@
     <t>Edit Current release, search is not working</t>
   </si>
   <si>
-    <t>PDF is not generated and flow is breaking</t>
-  </si>
-  <si>
     <t>Admin is not able to see the reports for requests if he selects nothing.</t>
   </si>
   <si>
+    <t>in IE</t>
+  </si>
+  <si>
     <t>AddTeam manually, fireld mismatch from excel</t>
   </si>
   <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Expertise field is mandatory and not marked</t>
+  </si>
+  <si>
+    <t>New/Open</t>
+  </si>
+  <si>
+    <t>Add module by excel, Validations for submit button are not there, flow breaks.</t>
+  </si>
+  <si>
+    <t>PDF is not generated in roll off process</t>
+  </si>
+  <si>
+    <t>PDF is generated in the name of the previous username or the username we used first.</t>
+  </si>
+  <si>
+    <t>Add module by excel, the user is unable to insert new modules and flow breaks</t>
+  </si>
+  <si>
+    <t>Add team by excel, if the user enters wrong sheet no., the flow breaks</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Open/In Progress</t>
+  </si>
+  <si>
+    <t>Fixed/Retest</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Sev 1</t>
+  </si>
+  <si>
+    <t>Sev 2</t>
+  </si>
+  <si>
+    <t>Sev 3</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>fixed</t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>open</t>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -190,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,12 +248,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -244,11 +293,220 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -275,15 +533,49 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,7 +850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,7 +861,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,39 +877,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -662,7 +954,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5">
@@ -678,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -687,13 +979,15 @@
         <v>12</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="12" t="s">
-        <v>45</v>
+      <c r="F6" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G6" s="5">
         <v>42234</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="8">
+        <v>42235</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -701,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
@@ -710,59 +1004,65 @@
         <v>12</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="9" t="s">
-        <v>44</v>
+      <c r="F7" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="G7" s="8">
         <v>42234</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8">
+        <v>42235</v>
+      </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="8">
-        <v>42234</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="D8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="31">
+        <v>42234</v>
+      </c>
+      <c r="H8" s="31">
+        <v>42235</v>
+      </c>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
+      <c r="F9" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G9" s="8">
         <v>42234</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="8">
+        <v>42235</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -770,24 +1070,26 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>14</v>
+      <c r="F10" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G10" s="8">
         <v>42234</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="8">
+        <v>42235</v>
+      </c>
       <c r="I10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -795,17 +1097,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>14</v>
+      <c r="F11" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G11" s="8">
         <v>42234</v>
@@ -818,24 +1120,24 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>14</v>
+      <c r="F12" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G12" s="8">
         <v>42234</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -843,22 +1145,24 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>44</v>
+      <c r="F13" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G13" s="8">
         <v>42234</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="8">
+        <v>42235</v>
+      </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -866,113 +1170,115 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G14" s="8">
         <v>42234</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="8">
+        <v>42234</v>
+      </c>
+      <c r="H15" s="8">
+        <v>42234</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="8">
-        <v>42234</v>
-      </c>
-      <c r="H15" s="8">
-        <v>42234</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>14</v>
+      <c r="F16" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G16" s="8">
         <v>42234</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
         <v>13</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="8">
-        <v>42234</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="D17" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="31">
+        <v>42234</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="12" t="s">
-        <v>44</v>
+      <c r="F18" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G18" s="8">
         <v>42234</v>
@@ -984,18 +1290,18 @@
       <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>35</v>
+      <c r="B19" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G19" s="8">
         <v>42234</v>
@@ -1003,22 +1309,22 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G20" s="8">
         <v>42234</v>
@@ -1026,22 +1332,22 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G21" s="8">
         <v>42234</v>
@@ -1054,17 +1360,17 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="12" t="s">
-        <v>45</v>
+      <c r="F22" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G22" s="8">
         <v>42234</v>
@@ -1072,50 +1378,52 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+    <row r="23" spans="1:9" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="30">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="8">
-        <v>42234</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="B23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="31">
+        <v>42234</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>14</v>
+      <c r="F24" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G24" s="8">
         <v>42234</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="8">
+        <v>42235</v>
+      </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1123,22 +1431,24 @@
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="12" t="s">
-        <v>45</v>
+      <c r="F25" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G25" s="8">
         <v>42234</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="8">
+        <v>42235</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1146,40 +1456,44 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>14</v>
+      <c r="F26" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="G26" s="8">
         <v>42234</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="H26" s="8">
+        <v>42235</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>14</v>
+      <c r="F27" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="G27" s="8">
         <v>42234</v>
@@ -1187,47 +1501,97 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="8">
+        <v>42235</v>
+      </c>
       <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="8">
+        <v>42235</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="8">
+        <v>42235</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>27</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="8">
+        <v>42235</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
@@ -1309,10 +1673,150 @@
       <c r="I38" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:I31"/>
   <mergeCells count="2">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E6:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="17">
+        <v>4</v>
+      </c>
+      <c r="G9" s="10">
+        <v>9</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>9</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="18">
+        <v>6</v>
+      </c>
+      <c r="G13" s="12">
+        <v>19</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2</v>
+      </c>
+      <c r="I13" s="13">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>